<commit_message>
chinh sua datafeed, them thiet ke warehouse
</commit_message>
<xml_diff>
--- a/docs/Data Feed Specification.xlsx
+++ b/docs/Data Feed Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DWProject\WH_Nhom9_DongHo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BB8D92-8990-4C7D-95B4-2FE1626973C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C499C64-BE4F-4194-94D3-E620C90CE3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{751DF043-DEDB-4487-BBC2-F5CA996CB508}"/>
   </bookViews>
@@ -226,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +246,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -280,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -292,6 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -610,7 +618,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,8 +706,8 @@
       <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>8</v>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>6</v>
@@ -712,8 +720,8 @@
       <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>48</v>
+      <c r="M3" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -728,8 +736,8 @@
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>9</v>
@@ -742,8 +750,8 @@
       <c r="L4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>49</v>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>